<commit_message>
Fix for units Text/Speaker in single corpus analysis, cmp does not work for now
</commit_message>
<xml_diff>
--- a/data_xlsx/PTAn.xlsx
+++ b/data_xlsx/PTAn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maciejuberna/Dev/PTAn/data_xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916D9995-2616-6D4E-BE6B-3F9CAD0162C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB044CA-8076-174D-A12D-81DE1FAB776F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US2016G1tvPTA" sheetId="1" r:id="rId1"/>
@@ -13436,8 +13436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21391,7 +21391,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M867"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -21399,8 +21401,8 @@
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="17.5" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="10" width="17.83203125" customWidth="1"/>

</xml_diff>